<commit_message>
added other hyperparameter results
</commit_message>
<xml_diff>
--- a/Hyper Parameter Results.xlsx
+++ b/Hyper Parameter Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI Laptop\Desktop\Code\Python\Jupyter Notebook\Thesis 2024 U.S. Presidential Election Sentiment Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B38B532-49D5-4ECB-AAA5-97D76C92238A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0221532D-563A-4229-92AD-CCFB8A2289B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0E+00"/>
+    <numFmt numFmtId="164" formatCode="0E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -114,12 +114,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -136,6 +136,12 @@
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -433,15 +439,28 @@
     <col min="5" max="5" width="8.88671875" style="6"/>
     <col min="6" max="8" width="8.88671875" style="3"/>
     <col min="9" max="9" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -466,8 +485,32 @@
       <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
@@ -477,23 +520,47 @@
       <c r="C3" s="5">
         <v>16</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="8">
         <v>0.69364664926022601</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="9">
         <v>0.85233128733105101</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="9">
         <v>0.68452564921087999</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="9">
         <v>0.68411005265992797</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="9">
         <v>0.69364664926022601</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J3" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5">
+        <v>32</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0.68146214099216695</v>
+      </c>
+      <c r="N3" s="9">
+        <v>0.76395166416962901</v>
+      </c>
+      <c r="O3" s="9">
+        <v>0.67615669444555004</v>
+      </c>
+      <c r="P3" s="9">
+        <v>0.69068371008503004</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>0.68146214099216695</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3.0000000000000001E-5</v>
       </c>
@@ -503,23 +570,47 @@
       <c r="C4" s="5">
         <v>32</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="8">
         <v>0.70234986945169697</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="9">
         <v>0.81125626133547801</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="9">
         <v>0.70859025713081802</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="9">
         <v>0.72423409223425705</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="9">
         <v>0.70234986945169697</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J4" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" s="5">
+        <v>32</v>
+      </c>
+      <c r="M4" s="8">
+        <v>0.69538729329852</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0.76935780296723</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0.69065368770299795</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0.68883261066568802</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>0.69538729329852</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4.0000000000000003E-5</v>
       </c>
@@ -529,157 +620,232 @@
       <c r="C5" s="5">
         <v>32</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="8">
         <v>0.71540469973890297</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="9">
         <v>1.1379542383882699</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="9">
         <v>0.71880727293132096</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="9">
         <v>0.72479653085152795</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="9">
         <v>0.71540469973890297</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J5" s="2">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2</v>
+      </c>
+      <c r="L5" s="5">
+        <v>32</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0.69799825935596105</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0.73892900513278104</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0.69909563298247102</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0.71023540726565704</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>0.69799825935596105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D6" s="7"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="J6" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="K6" s="3">
+        <v>3</v>
+      </c>
+      <c r="L6" s="5">
+        <v>16</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0.71714534377719696</v>
+      </c>
+      <c r="N6" s="9">
+        <v>0.87437102219296803</v>
+      </c>
+      <c r="O6" s="9">
+        <v>0.71170087876424204</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0.71130672220174396</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0.71714534377719696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J7" s="2">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="5">
+        <v>32</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0.71801566579634402</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0.81000777499543297</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0.71604160463822497</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0.71616392262700201</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0.71801566579634402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J8" s="2">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="K8" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="5">
-        <v>16</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0.67362924281984304</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0.82945016730162802</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0.67868711760860001</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0.692552902661973</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0.67362924281984304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="L8" s="5">
+        <v>32</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.70670147954743201</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0.755784278114636</v>
+      </c>
+      <c r="O8" s="9">
+        <v>0.69497139849516298</v>
+      </c>
+      <c r="P8" s="9">
+        <v>0.69739551632010999</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>0.70670147954743201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J9" s="2">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="B10" s="3">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5">
-        <v>32</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.67885117493472502</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.96701505200730398</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0.68228426094511796</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0.69568085027563697</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0.67885117493472502</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="K9" s="3">
+        <v>3</v>
+      </c>
+      <c r="L9" s="5">
+        <v>32</v>
+      </c>
+      <c r="M9" s="8">
+        <v>0.68320278503046095</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0.87845367689927401</v>
+      </c>
+      <c r="O9" s="9">
+        <v>0.68418047287309502</v>
+      </c>
+      <c r="P9" s="9">
+        <v>0.68552395061328497</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>0.68320278503046095</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J10" s="2">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="B11" s="3">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5">
-        <v>32</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0.68059181897302001</v>
-      </c>
-      <c r="E11" s="6">
-        <v>1.2956163502401701</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0.68680485009665304</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.70217432191699702</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0.68059181897302001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K10" s="3">
+        <v>2</v>
+      </c>
+      <c r="L10" s="5">
+        <v>32</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0.69364664926022601</v>
+      </c>
+      <c r="N10" s="9">
+        <v>0.74011119537883296</v>
+      </c>
+      <c r="O10" s="9">
+        <v>0.70129975963187696</v>
+      </c>
+      <c r="P10" s="9">
+        <v>0.72085063367423796</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>0.69364664926022601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J11" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3</v>
+      </c>
+      <c r="L11" s="5">
+        <v>32</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0.69625761531766694</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0.87522508203983296</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0.68508116014718301</v>
+      </c>
+      <c r="P11" s="9">
+        <v>0.68471409955132301</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0.69625761531766694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D12" s="7"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D13" s="7"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -704,228 +870,335 @@
       <c r="H14" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>1.0000000000000001E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
       </c>
       <c r="C15" s="5">
-        <v>32</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0.68146214099216695</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0.76395166416962901</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0.67615669444555004</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0.69068371008503004</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0.68146214099216695</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.67362924281984304</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.82945016730162802</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0.67868711760860001</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.692552902661973</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.67362924281984304</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K15" s="3">
+        <v>5</v>
+      </c>
+      <c r="L15" s="5">
+        <v>32</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0.66753698868581302</v>
+      </c>
+      <c r="N15" s="9">
+        <v>0.93434653927882505</v>
+      </c>
+      <c r="O15" s="9">
+        <v>0.67110644602084601</v>
+      </c>
+      <c r="P15" s="9">
+        <v>0.68321254360706096</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>0.66753698868581302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5">
+        <v>32</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.67885117493472502</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.96701505200730398</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.68228426094511796</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0.69568085027563697</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.67885117493472502</v>
+      </c>
+      <c r="J16" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="B16" s="3">
-        <v>3</v>
-      </c>
-      <c r="C16" s="5">
-        <v>32</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0.69538729329852</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0.76935780296723</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0.69065368770299795</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0.68883261066568802</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0.69538729329852</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K16" s="3">
+        <v>2</v>
+      </c>
+      <c r="L16" s="5">
+        <v>32</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.67711053089643103</v>
+      </c>
+      <c r="N16" s="9">
+        <v>0.76842873212363905</v>
+      </c>
+      <c r="O16" s="9">
+        <v>0.67175795474178202</v>
+      </c>
+      <c r="P16" s="9">
+        <v>0.66997783499008601</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>0.67711053089643103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="B17" s="3">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>32</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.68059181897302001</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1.2956163502401701</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0.68680485009665304</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0.70217432191699702</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0.68059181897302001</v>
+      </c>
+      <c r="J17" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="B17" s="3">
+      <c r="K17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="5">
-        <v>32</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0.69799825935596105</v>
-      </c>
-      <c r="E17" s="6">
-        <v>0.73892900513278104</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0.69909563298247102</v>
-      </c>
-      <c r="G17" s="6">
-        <v>0.71023540726565704</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0.69799825935596105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="L17" s="5">
+        <v>32</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0.68320278503046095</v>
+      </c>
+      <c r="N17" s="9">
+        <v>0.75432007014751401</v>
+      </c>
+      <c r="O17" s="9">
+        <v>0.68281244773928595</v>
+      </c>
+      <c r="P17" s="9">
+        <v>0.68328239639872601</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>0.68320278503046095</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J18" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="B18" s="3">
-        <v>3</v>
-      </c>
-      <c r="C18" s="5">
-        <v>32</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0.71801566579634402</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0.81000777499543297</v>
-      </c>
-      <c r="F18" s="6">
-        <v>0.71604160463822497</v>
-      </c>
-      <c r="G18" s="6">
-        <v>0.71616392262700201</v>
-      </c>
-      <c r="H18" s="6">
-        <v>0.71801566579634402</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="7"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="B22" s="3">
-        <v>5</v>
-      </c>
-      <c r="C22" s="5">
-        <v>32</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.66753698868581302</v>
-      </c>
-      <c r="E22" s="6">
-        <v>0.93434653927882505</v>
-      </c>
-      <c r="F22" s="6">
-        <v>0.67110644602084601</v>
-      </c>
-      <c r="G22" s="6">
-        <v>0.68321254360706096</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0.66753698868581302</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="B23" s="3">
+      <c r="K18" s="3">
+        <v>3</v>
+      </c>
+      <c r="L18" s="5">
+        <v>16</v>
+      </c>
+      <c r="M18" s="8">
+        <v>0.67885117493472502</v>
+      </c>
+      <c r="N18" s="9">
+        <v>0.90440371901624705</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0.68057273513474803</v>
+      </c>
+      <c r="P18" s="9">
+        <v>0.68466384474521802</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>0.67885117493472502</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J19" s="2">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3</v>
+      </c>
+      <c r="L19" s="5">
+        <v>32</v>
+      </c>
+      <c r="M19" s="8">
+        <v>0.67798085291557797</v>
+      </c>
+      <c r="N19" s="9">
+        <v>0.80893432762887696</v>
+      </c>
+      <c r="O19" s="9">
+        <v>0.68191729575933202</v>
+      </c>
+      <c r="P19" s="9">
+        <v>0.69141388318916097</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>0.67798085291557797</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J20" s="2">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="K20" s="3">
         <v>2</v>
       </c>
-      <c r="C23" s="5">
-        <v>32</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0.67711053089643103</v>
-      </c>
-      <c r="E23" s="6">
-        <v>0.76842873212363905</v>
-      </c>
-      <c r="F23" s="6">
-        <v>0.67175795474178202</v>
-      </c>
-      <c r="G23" s="6">
-        <v>0.66997783499008601</v>
-      </c>
-      <c r="H23" s="6">
-        <v>0.67711053089643103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="B24" s="3">
+      <c r="L20" s="5">
+        <v>32</v>
+      </c>
+      <c r="M20" s="8">
+        <v>0.67188859878154905</v>
+      </c>
+      <c r="N20" s="9">
+        <v>0.74695446673366706</v>
+      </c>
+      <c r="O20" s="9">
+        <v>0.67689719020205597</v>
+      </c>
+      <c r="P20" s="9">
+        <v>0.687682409524491</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>0.67188859878154905</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J21" s="2">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+      <c r="L21" s="5">
+        <v>32</v>
+      </c>
+      <c r="M21" s="8">
+        <v>0.66579634464751902</v>
+      </c>
+      <c r="N21" s="9">
+        <v>0.91638502892520601</v>
+      </c>
+      <c r="O21" s="9">
+        <v>0.67662286513092396</v>
+      </c>
+      <c r="P21" s="9">
+        <v>0.70588283528600004</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>0.66579634464751902</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J22" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="K22" s="3">
         <v>2</v>
       </c>
-      <c r="C24" s="5">
-        <v>32</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0.68320278503046095</v>
-      </c>
-      <c r="E24" s="6">
-        <v>0.75432007014751401</v>
-      </c>
-      <c r="F24" s="6">
-        <v>0.68281244773928595</v>
-      </c>
-      <c r="G24" s="6">
-        <v>0.68328239639872601</v>
-      </c>
-      <c r="H24" s="6">
-        <v>0.68320278503046095</v>
+      <c r="L22" s="5">
+        <v>32</v>
+      </c>
+      <c r="M22" s="8">
+        <v>0.69451697127937295</v>
+      </c>
+      <c r="N22" s="9">
+        <v>0.76035804301500298</v>
+      </c>
+      <c r="O22" s="9">
+        <v>0.69121840422337399</v>
+      </c>
+      <c r="P22" s="9">
+        <v>0.68925283247633395</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>0.69451697127937295</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J23" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="K23" s="3">
+        <v>3</v>
+      </c>
+      <c r="L23" s="5">
+        <v>32</v>
+      </c>
+      <c r="M23" s="8">
+        <v>0.66579634464751902</v>
+      </c>
+      <c r="N23" s="9">
+        <v>0.92361577434672204</v>
+      </c>
+      <c r="O23" s="9">
+        <v>0.66539871693988195</v>
+      </c>
+      <c r="P23" s="9">
+        <v>0.68291234725374905</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>0.66579634464751902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>